<commit_message>
armor_list excel 파일 일부 수정
</commit_message>
<xml_diff>
--- a/app/armor_list.xlsx
+++ b/app/armor_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="590" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Armor" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="2178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2263" uniqueCount="2263">
   <si>
     <t>레더헤드</t>
   </si>
@@ -6552,6 +6552,261 @@
   </si>
   <si>
     <t>흔들흔들 티켓</t>
+  </si>
+  <si>
+    <t>(2)둔기 사용 : 예리도가 나쁠수록 공격력 상승. 원거리 무기의 근접공격 위력과 기절시킬 확률이 매우 크게 상승./(4)무속성 강화 : 장비 중인 무속성 무기를 강화한다.</t>
+  </si>
+  <si>
+    <t>(3)둔기 사용 : 예리도가 나쁠수록 공격력 상승.  원거리 무기의 근접공격 위력과 기절시킬 확률이 매우 크게 상승.</t>
+  </si>
+  <si>
+    <t>(2)분발 : 체력이 40% 이하가 되면 일정 시간 스태미나 소비량이 감소한다./(4)스태미나 한계 돌파 : 스태미나의 한계치가 증가한다.</t>
+  </si>
+  <si>
+    <t>(2)둔기 사용 : 예리도가 나쁠수록 공격력 상승. / 원거리 무기의 근접공격 위력과 기절시킬 확률이 매우 크게 상승.|(4)무속성 강화 : 장비 중인 무속성 무기를 강화한다.</t>
+  </si>
+  <si>
+    <t>(2)분발 : 체력이 40% 이하가 되면 일정 시간 스태미나 소비량이 감소한다.|(4)스태미나 한계 돌파 : 스태미나의 한계치가 증가한다.</t>
+  </si>
+  <si>
+    <t>(2)스태미나 한계 돌파 : 스태미나의 한계치가 증가한다.|(4)심안/탄도 강화 : 공격이 튕겨 나가지 않는다. / 탄과 화살이 최대 위력이 되기까지의 거리가 짧아진다.</t>
+  </si>
+  <si>
+    <t>(2)비연 [속성] : 점프 공격의 속성 대미지 UP|(4)달인의 재주 : 회심 발생 시 예리도가 소모되지 않는다.</t>
+  </si>
+  <si>
+    <t>(2)발도술 [힘] : 무기 발도 공격에 기절을 유발하는 힘이 추가 및 강화되며 공격력도 약간 오른다.|(4)칼날 연마 : 무기를 연마하면, 일정 시간 동안 예리도가 떨어지지 않는다.</t>
+  </si>
+  <si>
+    <t>(2)행운 : 퀘스트 클리어로 받는 보수의 수가 늘어날 확률이 높아진다. (퀘스트 도중에는 효과를 얻을 수 없음)|(4)활 모으기 단계 해제 : 활의 모으기 단계가 1단계 증가.</t>
+  </si>
+  <si>
+    <t>(2)회심격 [속성] : 공격으로 회심이 발생했을 때 주는 속성 데미지 (불, 물, 번개, 얼음, 용)가 높아진다.|(4)심안/탄도 강화 : 공격이 튕겨 나가지 않는다. / 탄과 화살이 최대 위력이 되기까지의 거리가 짧아진다.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 일부 아이템을 사용했을 때 효과의 1/3을 주위 동료에게도 준다.|Lv.2 : 일부 아이템을 사용했을 때 효과의 1/3을 넓은 범위의 동료에게도 준다.|Lv.3 : 일부 아이템을 사용했을 때 효과의 2/3을 넓은 범위의 동료에게도 준다.|Lv.4 : 일부 아이템을 사용했을 때 효과의 2/3을 꽤 넓은 범위의 동료에게도 준다.|Lv.5 : 일부 아이템을 사용했을 때 동일한 효과를 꽤 넓은 범위의 동료에게도 준다.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 속도가 조금 상승한다.|Lv.2 : 속도가 상승한다.|Lv.3 : 속도가 많이 상승한다.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 동반자의 공격력과 방어력이 1.05배|Lv.2 : 동반자의 공격력과 방어력이 1.1배|Lv.3 : 동반자의 공격력과 방어력이 1.15배|Lv.4 : 동반자의 공격력과 방어력이 1.2배|Lv.5 : 동반자의 공격력과 방어력이 1.25배</t>
+  </si>
+  <si>
+    <t>Lv.1 : 면 포자풀 사용시 체력을 20 회복한다.|Lv.2 : 면 포자풀 사용시 체력을 35 회복한다.|Lv.3 : 면 포자풀 사용시 체력을 60 회복한다.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 푸른 버섯과 독광대버섯을 먹을 수 있게 되며 좋은 효과를 얻을 수 있다|Lv.2 : 추가로 니트로 버섯, 마비 버섯을 먹을 수 있게 되며 좋은 효과를 얻을 수 있다|Lv.3 : 추가로 만드라고라, 도깨비 니트로버섯, 두근두근 버섯을 먹을 수 있게 되며 좋은 효과를 얻을 수 있다</t>
+  </si>
+  <si>
+    <t>Lv.1 : 먹는 속도가 조금 상승한다|Lv.2 : 먹는 속도가 상승한다|Lv.3 : 먹는 속도가 많이 상승한다</t>
+  </si>
+  <si>
+    <t>Lv.1 : 지면이나 식물에서 획득할 수 있는 탄의 장전 수가 조금 증가한다|Lv.2 : 그리고 몬스터가 떨어뜨리는 일부 탄의 장전 수가 조금 증가한다|Lv.3 : 그리고 몬스터가 떨어뜨리는 모든 탄의 장전 수가 조금 증가한다</t>
+  </si>
+  <si>
+    <t>Lv.1 : 일부 아이템의 효과 시간  1.1배|Lv.2 : 일부 아이템의 효과 시간  1.25배|Lv.3 : 일부 아이템의 효과 시간  1.5배</t>
+  </si>
+  <si>
+    <t>Lv.1 : 들켜도 전투 상태가 될 확률이 낮다.|Lv.2 : 들켜도 전투 상태가 될 확률이 매우 낮다.|Lv.3 : 들켜도 전투 상태가 되지 않는다.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 몬스터에게서 은신에 성공 확률이 조금 증가한다.|Lv.2 : 몬스터에게서 은신에 성공 확률이 증가한다.|Lv.3 : 몬스터에게서 은신에 성공 확률이 많이 증가한다.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 특수 장비의 재사용 시간 5% 단축|Lv.2 : 특수 장비의 재사용 시간 10% 단축|Lv.3 : 특수 장비의 재사용 시간 20% 단축</t>
+  </si>
+  <si>
+    <t>Lv.1 : 물가에서 이동 속도 감소 없음.|Lv.2 : 물가에서 이동 속도가 감소하지 않으며 물가에서 회피 성능 향상.|Lv.3 : 물가에서 이동 속도가 감소하지 않으며 물가에서 회피 성능 크게 향상.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 대시 등 서서히 스태미나를 소모하는 행동의 스태미나 소모량 15% 감소|Lv.2 : 대시 등 서서히 스태미나를 소모하는 행동의 스태미나 소모량 30% 감소|Lv.3 : 대시 등 서서히 스태미나를 소모하는 행동의 스태미나 소모량 50% 감소</t>
+  </si>
+  <si>
+    <t>Lv.1 : 스태미나 게이지의 감소까지 걸리는 시간을 30% 연장.|Lv.2 : 스태미나 게이지의 감소까지 걸리는 시간을 60% 연장.Lv.3 : 시간 경과에 따른 스태미나 게이지의 감소 무효화.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 스태미나 게이지의 감소까지 걸리는 시간을 30% 연장.|Lv.2 : 스태미나 게이지의 감소까지 걸리는 시간을 60% 연장.|Lv.3 : 시간 경과에 따른 스태미나 게이지의 감소 무효화.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 스태미나 회복 속도 1.1배|Lv.2 : 스태미나 회복 속도 1.2배|Lv.3 : 스태미나 회복 속도 1.3배</t>
+  </si>
+  <si>
+    <t>Lv.1 : 회피 등 고정으로 스태미나가 소모되는 행동의 고정 스태미나 소모량 10% 감소|Lv.2 : 회피 등 고정으로 스태미나가 소모되는 행동의 고정 스태미나 소모량 20% 감소|Lv.3 : 회피 등 고정으로 스태미나가 소모되는 행동의 고정 스태미나 소모량 30% 감소|Lv.4 : 회피 등 고정으로 스태미나가 소모되는 행동의 고정 스태미나 소모량 40% 감소|Lv.5 : 회피 등 고정으로 스태미나가 소모되는 행동의 고정 스태미나 소모량 50% 감소</t>
+  </si>
+  <si>
+    <t>Lv.1 : 곤충종 소형 몬스터의 사체가 남는 확률이 상승한다|Lv.2 : 곤충종 소형 몬스터의 사체가 남는 확률이 상당히 상승한다|Lv.3 : 곤충종 소형 몬스터의 사체가 반드시 남는다</t>
+  </si>
+  <si>
+    <t>Lv.1 : 약초 등의 풀 계열 소비 아이템의 취득 수+1|Lv.2 : 추가로 열매나 씨앗 계열 소비 아이템의 취득 수+1|Lv.3 : 추가로 곤충 소비 아이템의 취득 수+1|Lv.4 : 추가로 버섯 소비 아이템의 취득 수+1</t>
+  </si>
+  <si>
+    <t>Lv.1 : 뼈 채취 포인트의 채취 횟수+1|Lv.2 : 추가로 특산품 채취 포인트의 채취 횟수+1|Lv.3 : 추가로 광석 채굴 포인트의 채취 횟수+1</t>
+  </si>
+  <si>
+    <t>Lv.1 : 공격의 위력을 조금 감소.|Lv.2 : 공격의 위력을 조금 감소.  스태미나 소모량을 15% 감소.|Lv.3 : 공격의 위력을 크게 감소.  스태미나 소모량을 15% 감소.|Lv.4 : 공격의 위력을 크게 감소.  스태미나 소모량을 30% 감소.|Lv.5 : 공격의 위력을 아주 크게 감소.  스태미나 소모량을 50% 감소.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 기절 상태의 시간을 30% 줄인다|Lv.2 : 기절 상태의 시간을 60% 줄인다|Lv.3 : 기절 상태가 되지 않는다</t>
+  </si>
+  <si>
+    <t>Lv.1 : 진동 [소]를 무효화한다|Lv.2 : 진동 [소]를 무효화하고 진동 [대]의 영향이 줄어든다.|Lv.3 : 진동 [소] [대]를 무효화한다</t>
+  </si>
+  <si>
+    <t>Lv.1 : 독 상태의 시간을 30% 줄인다|Lv.2 : 독 상태의 시간을 60% 줄인다|Lv.3 : 독 상태가 되지 않는다</t>
+  </si>
+  <si>
+    <t>Lv.1 : 독기의 침식을 억제한다.|Lv.2 : 독기의 침식을 많이 억제한다.|Lv.3 : 독기의 침식 상태를 무효화한다.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 마비 상태의 시간을 30% 줄인다|Lv.2 : 마비 상태의 시간을 60% 줄인다|Lv.3 : 마비 상태가 되지 않는다</t>
+  </si>
+  <si>
+    <t>Lv.1 : 물 내성+6|Lv.2 : 물 내성+12|Lv.3 : 물 내성+20, 방어력+10</t>
+  </si>
+  <si>
+    <t>Lv.1 : 방어력+5|Lv.2 : 방어력+10|Lv.3 : 방어력+15|Lv.4 : 방어력+20 , 모든 속성 내성치+3|Lv.5 : 방어력+25 , 모든 속성 내성치+3|Lv.6 : 방어력+30 , 모든 속성 내성치+3|Lv.7 : 방어력+35 , 모든 속성 내성치+3</t>
+  </si>
+  <si>
+    <t>Lv.1 : 방어력 DOWN 상태의 시간을 30% 줄인다.|Lv.2 : 방어력 DOWN 상태의 시간을 60% 줄인다.|Lv.3 : 방어력 DOWN 상태가 되지 않는다.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 번개 내성+6|Lv.2 : 번개 내성+12|Lv.3 : 번개 내성+20, 방어력+10</t>
+  </si>
+  <si>
+    <t>Lv.1 : 불 내성+6|Lv.2 : 불 내성+12|Lv.3 : 불 내성+20, 방어력+10</t>
+  </si>
+  <si>
+    <t>Lv.1 : 모든 속성 피해의 효과 시간을 30% 줄인다|Lv.2 : 모든 속성 피해의 효과 시간을 60% 줄인다|Lv.3 : 모든 속성 피해를 무효화한다.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 수면 상태의 시간을 30% 줄인다|Lv.2 : 수면 상태의 시간을 60% 줄인다|Lv.3 : 수면 상태가 되지 않는다</t>
+  </si>
+  <si>
+    <t>Lv.1 : 얼음 내성+6|Lv.2 : 얼음 내성+12|Lv.3 : 얼음 내성+20, 방어력+10</t>
+  </si>
+  <si>
+    <t>Lv.1 : 열상 상태에 의한 데미지를 경감한다|Lv.2 : 열상 상태에 의한 데미지를 크게 경감한다|Lv.3 : 열상 상태가 되지 않는다</t>
+  </si>
+  <si>
+    <t>Lv.1 : 용 내성+6|Lv.2 : 용 내성+12|Lv.3 : 용 내성+20, 방어력+10</t>
+  </si>
+  <si>
+    <t>Lv.1 : 움츠리지 않음.|Lv.2 : 움츠리지 않음. 엉덩방아를 움츠림으로 감소시킨다.|Lv.3 : 움츠림, 엉덩방아를 무효화</t>
+  </si>
+  <si>
+    <t>Lv.1 : 플레이어가 받는 데미지를 일정 확률로 15% 감소한다|Lv.2 : 플레이어가 받는 데미지를 일정 확률로 30% 감소한다|Lv.3 : 플레이어가 받는 데미지를 일정 확률로 50% 감소한다</t>
+  </si>
+  <si>
+    <t>Lv.1 : 체력+15|Lv.2 : 체력+30|Lv.3 : 체력+50</t>
+  </si>
+  <si>
+    <t>Lv.1 : 회복량 1.1배|Lv.2 : 회복량 1.2배|Lv.3 : 회복량 1.3배</t>
+  </si>
+  <si>
+    <t>Lv.1 : 폭파까지의 시간이 연장되고, 폭파 데미지가 줄어든다.|Lv.2 : 폭파까지의 시간이 더욱 연장되고, 폭파 데미지가 크게 줄어든다.|Lv.3 : 폭파 피해를 받지 않는다.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 풍압 [소]를 조금 줄인다|Lv.2 : 풍압 [소]를 줄인다|Lv.3 : 풍압 [소]를 무효화한다|Lv.4 : 풍압 [소]를 무효화하고 풍압 [대]를 줄인다|Lv.5 : 풍압 [대]를 무효화한다</t>
+  </si>
+  <si>
+    <t>Lv.1 : 붉은 게이지의 자동 회복 속도 2배|Lv.2 : 붉은 게이지의 자동 회복 속도 3배|Lv.3 : 붉은 게이지의 자동 회복 속도 4배</t>
+  </si>
+  <si>
+    <t>Lv.1 : 회피 거리가 조금 연장.|Lv.2 : 회피 거리가 연장.|Lv.3 : 회피 거리가 크게 연장.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 무적 시간이 아주 조금 연장.|Lv.2 : 무적 시간이 조금 연장.|Lv.3 : 무적 시간이 연장.|Lv.4 : 무적 시간이 크게 연장.|Lv.5 : 무적 시간이 아주 크게 연장.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 몬스터에 대한 공격의 기절 위력이 1.1배|Lv.2 : 몬스터에 대한 공격의 기절 위력이 1.2배|Lv.3 : 몬스터에 대한 공격의 기절 위력이 1.3배</t>
+  </si>
+  <si>
+    <t>Lv.1 : 회심률+3%|Lv.2 : 회심률+6%|Lv.3 : 회심률+10%|Lv.4 : 회심률+15%|Lv.5 : 회심률+20%|Lv.6 : 회심률+25%|Lv.7 : 회심률+30%</t>
+  </si>
+  <si>
+    <t>Lv.1 : 태도, 쌍검, 조충곤, 슬래시 액스, 차지 액스의 강화 상태 지속 시간 1.1배|Lv.2 : 태도, 쌍검, 조충곤, 슬래시 액스, 차지 액스의 강화 상태 지속 시간 1.2배|Lv.3 : 태도, 쌍검, 조충곤, 슬래시 액스, 차지 액스의 강화 상태 지속 시간 1.3배</t>
+  </si>
+  <si>
+    <t>Lv.1 : 기초 공격력+3|Lv.2 : 기초 공격력+6|Lv.3 : 기초 공격력+9|Lv.4 : 기초 공격력+12, 회심률+5％|Lv.5 : 기초 공격력+15, 회심률+5%|Lv.6 : 기초 공격력+18, 회심률+5%|Lv.7 : 기초 공격력+21, 회심률+5%</t>
+  </si>
+  <si>
+    <t>Lv.1 : 대형 몬스터 분노시 기초 공격력+4 회심률+3%|Lv.2 : 대형 몬스터 분노시 기초 공격력+8 회심률+6%|Lv.3 : 대형 몬스터 분노시 기초 공격력+12 회심률+9%|Lv.4 : 대형 몬스터 분노시 기초 공격력+16 회심률+12%|Lv.5 : 대형 몬스터 분노시 기초 공격력+20 회심률+15%</t>
+  </si>
+  <si>
+    <t>Lv.1 : 독 축적치가 1.05배가 되고 독의 축적치에+10|Lv.2 : 독 축적치가 1.1배가 되고 독의 축적치에+10|Lv.3 : 독 축적치가 1.2배가 되고 독의 축적치에+10</t>
+  </si>
+  <si>
+    <t>Lv.1 : 마비 축적치가 1.05배가 되고 마비의 축적치에+10|Lv.2 : 마비 축적치가 1.1배가 되고 마비의 축적치에+10|Lv.3 : 마비 축적치가 1.2배가 되고 마비의 축적치에+10</t>
+  </si>
+  <si>
+    <t>Lv.1 : 물속성 공격치+30|Lv.2 : 물속성 공격치+60|Lv.3 : 물속성 공격치+100|Lv.4 : 물속성 공격치가 1.05배가 되고 물속성 공격치+100|Lv.5 : 물속성 공격치가 1.1배가 되고 물속성 공격치+100</t>
+  </si>
+  <si>
+    <t>Lv.1 : 발도 공격 회심률+30%|Lv.2 : 발도 공격 회심률+60%|Lv.3 : 발도 공격 회심률+100%</t>
+  </si>
+  <si>
+    <t>Lv.1 : 번개속성 공격치+30|Lv.2 : 번개속성 공격치+60|Lv.3 : 번개속성 공격치+100|Lv.4 : 번개속성 공격치가 1.05배가 되고 번개속성 공격치+100|Lv.5 : 번개속성 공격치가 1.1배가 되고 번개속성 공격치+100</t>
+  </si>
+  <si>
+    <t>Lv.1 : 폭탄 계열 아이템의 위력 1.1배|Lv.2 : 폭탄 계열 아이템의 위력 1.2배|Lv.3 : 폭탄 계열 아이템의 위력 1.3배</t>
+  </si>
+  <si>
+    <t>Lv.1 : 불속성 공격치+30|Lv.2 : 불속성 공격치+60|Lv.3 : 불속성 공격치+100|Lv.4 : 불속성 공격치가 1.05배가 되고, 불속성 공격치에+100|Lv.5 : 불속성 공격치가 1.1배가 되고, 불속성 공격치에+100</t>
+  </si>
+  <si>
+    <t>Lv.1 : 숨은 속성의 1/3을 이끌어낸다. / 일부 탄의 장전 수 증가.|Lv.2 : 숨은 속성의 2/3을 이끌어낸다. / 여러 탄의 장전 수 증가.|Lv.3 : 숨은 속성을 100% 이끌어낸다. / 거의 모든 탄의 장전 수 증가.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 수면 축적치가 1.05배가 되고 수면의 축적치에+10|Lv.2 : 수면 축적치가 1.1배가 되고 수면의 축적치에+10|Lv.3 : 수면 축적치가 1.2배가 되고 수면의 축적치에+10</t>
+  </si>
+  <si>
+    <t>Lv.1 : 연마 동작을 1회 생략.|Lv.2 : 연마 동작을 2회 생략.|Lv.3 : 연마 동작을 3회 생략.</t>
+  </si>
+  <si>
+    <t>Lv.1 : 회심 공격 시의 데미지 배율 1.3배|Lv.2 : 회심 공격 시의 데미지 배율 1.35배|Lv.3 : 회심 공격 시의 데미지 배율 1.4배</t>
+  </si>
+  <si>
+    <t>Lv.1 : 기력 감소 위력 1.1배|Lv.2 : 기력 감소 위력 1.2배|Lv.3 : 기력 감소 위력 1.3배</t>
+  </si>
+  <si>
+    <t>Lv.1 : 체력 게이지에 빨간 부분이 있는 동안 기초 공격력+5|Lv.2 : 체력 게이지에 빨간 부분이 있는 동안 기초 공격력+10|Lv.3 : 체력 게이지에 빨간 부분이 있는 동안 기초 공격력+15|Lv.4 : 체력 게이지에 빨간 부분이 있는 동안 기초 공격력+20|Lv.5 : 체력 게이지에 빨간 부분이 있는 동안 기초 공격력+25</t>
+  </si>
+  <si>
+    <t>Lv.1 : 얼음 속성 공격치+30|Lv.2 : 얼음 속성 공격치+60|Lv.3 : 얼음 속성 공격치+100|Lv.4 : 얼음 속성 공격치가 1.05배가 되고 얼음 속성 공격치+100|Lv.5 : 얼음 속성 공격치가 1.1배가 되고 얼음 속성 공격치+100</t>
+  </si>
+  <si>
+    <t>Lv.1 : 체력이 최대일때 기초 공격력+5|Lv.2 : 체력이 최대일때 기초 공격력+10|Lv.3 : 체력이 최대일때 기초 공격력+20</t>
+  </si>
+  <si>
+    <t>Lv.1 : 용속성 공격치+30|Lv.2 : 용속성 공격치+60|Lv.3 : 용속성 공격치+100|Lv.4 : 용속성 공격치가 1.05배가 되고 용속성 공격치+100|Lv.5 : 용속성 공격치가 1.1배가 되고 용속성 공격치+100</t>
+  </si>
+  <si>
+    <t>Lv.1 : 무기의 예리도+10|Lv.2 : 무기의 예리도+20|Lv.3 : 무기의 예리도+30|Lv.4 : 무기의 예리도+40|Lv.5 : 무기의 예리도+50</t>
+  </si>
+  <si>
+    <t>Lv.1 : 체력이 최대치의 35% 이하일 때 공격력1.05배, 방어력+15|Lv.2 : 체력이 최대치의 35% 이하일 때 공격력1.1배, 방어력+20|Lv.3 : 체력이 최대치의 35% 이하일 때 공격력1.15배, 방어력+25|Lv.4 : 체력이 최대치의 35% 이하일 때 공격력1.2배, 방어력+30|Lv.5 : 체력이 최대치의 35% 이하일 때 공격력1.3배, 방어력+40</t>
+  </si>
+  <si>
+    <t>Lv.1 : 태도, 쌍검, 슬래시 액스, 차지 액스의 게이지 상승률 5% UP / 대검, 해머, 활의 모으는 시간 5% 단축|Lv.2 : 태도, 쌍검, 슬래시 액스, 차지 액스의 게이지 상승률 10% UP / 대검, 해머, 활의 모으는 시간 10% 단축|Lv.3 : 태도, 쌍검, 슬래시 액스, 차지 액스의 게이지 상승률 20% UP / 대검, 해머, 활의 모으는 시간 20% 단축</t>
+  </si>
+  <si>
+    <t>Lv.1 : 보우건의 특수탄과 활의 용화살의 위력이 1.1배|Lv.2 : 보우건의 특수탄과 활의 용화살의 위력이 1.2배</t>
+  </si>
+  <si>
+    <t>Lv.1 : 부위에 대한 축적 데미지 1.1배|Lv.2 : 부위에 대한 축적 데미지 1.2배|Lv.3 : 부위에 대한 축적 데미지 1.3배</t>
+  </si>
+  <si>
+    <t>Lv.1 : 건랜스의 포격, 용격포와 차지액스의 병공격, 철갑유탄 등 폭발 공격의 위력이 1.1배, 용격포의 냉각시간이 15% 감소|Lv.2 : 건랜스의 포격, 용격포와 차지액스의 병공격, 철갑유탄 등 폭발 공격의 위력이 1.2배, 용격포의 냉각시간이 30% 감소|Lv.3 : 건랜스의 포격, 용격포와 차지액스의 병공격, 철갑유탄 등 폭발 공격의 위력이 1.3배, 용격포의 냉각시간이 50% 감소</t>
+  </si>
+  <si>
+    <t>Lv.1 : 폭파 축적치가 1.05배가 되고 폭파의 축적치에+10|Lv.2 : 폭파 축적치가 1.1배가 되고 폭파의 축적치에+10|Lv.3 : 폭파 축적치가 1.2배가 되고 폭파의 축적치에+10</t>
+  </si>
+  <si>
+    <t>Lv.1 : 스태미나 게이지가 가득 차있을 경우 회심률+10%|Lv.2 : 스태미나 게이지가 가득 차있을 경우 회심률+20%|Lv.3 : 스태미나 게이지가 가득 차있을 경우 회심률+30%</t>
+  </si>
+  <si>
+    <t>Lv.1 : 특정 조건에서 회심률 +10% 스태미나 소비량 10% 감소|Lv.2 : 특정 조건에서 회심률 +20% 스태미나 소비량 20% 감소|Lv.3 : 특정 조건에서 회심률 +30% 스태미나 소비량 30% 감소|Lv.4 : 특정 조건에서 회심률 +40% 스태미나 소비량 40% 감소|Lv.5 : 특정 조건에서 회심률 +50% 스태미나 소비량 50% 감소</t>
   </si>
 </sst>
 </file>
@@ -6870,9 +7125,7 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -6887,9 +7140,7 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -6898,9 +7149,7 @@
       <bottom style="thick">
         <color theme="4"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -6909,9 +7158,7 @@
       <bottom style="thick">
         <color rgb="FFACCCEA"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -6920,9 +7167,7 @@
       <bottom style="medium">
         <color theme="4" tint="0.399980"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -6937,9 +7182,7 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -6954,9 +7197,7 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="double">
@@ -6971,9 +7212,7 @@
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -6982,9 +7221,7 @@
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -6995,9 +7232,7 @@
       <bottom style="double">
         <color theme="4"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
@@ -7377,17 +7612,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L753"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.250000" customHeight="1"/>
   <cols>
-    <col min="6" max="6" style="1" width="17.67166731" customWidth="1" outlineLevel="0"/>
-    <col min="7" max="7" style="1" width="19.67166731" customWidth="1" outlineLevel="0"/>
-    <col min="8" max="8" style="1" width="9.00500033" customWidth="1" outlineLevel="0"/>
-    <col min="10" max="10" style="1" width="9.00500033" customWidth="1" outlineLevel="0"/>
-    <col min="12" max="12" style="1" width="41.44944594" customWidth="1" outlineLevel="0"/>
+    <col min="6" max="6" style="1" width="17.71928488" customWidth="1" outlineLevel="0"/>
+    <col min="7" max="7" style="1" width="19.71928488" customWidth="1" outlineLevel="0"/>
+    <col min="8" max="8" style="1" width="9.00499998" customWidth="1" outlineLevel="0"/>
+    <col min="10" max="10" style="1" width="9.00499998" customWidth="1" outlineLevel="0"/>
+    <col min="12" max="12" style="1" width="41.43356977" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -26979,18 +27214,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="B112" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.250000" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="16.14785753" customWidth="1" outlineLevel="0"/>
+    <col min="2" max="2" width="255.71929060" customWidth="1" outlineLevel="0"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="0" t="s">
         <v>1402</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1403</v>
+        <v>2181</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -27022,7 +27261,7 @@
         <v>1410</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>1411</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -27070,7 +27309,7 @@
         <v>1422</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>1423</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -27086,7 +27325,7 @@
         <v>1426</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>1427</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -27102,7 +27341,7 @@
         <v>1430</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>1431</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -27134,7 +27373,7 @@
         <v>1438</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>1439</v>
+        <v>2186</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -27150,7 +27389,7 @@
         <v>1442</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>1443</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -27190,7 +27429,7 @@
         <v>1452</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>1453</v>
+        <v>2188</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -27198,7 +27437,7 @@
         <v>1454</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>1455</v>
+        <v>2189</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -27214,7 +27453,7 @@
         <v>1458</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>1459</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -27246,7 +27485,7 @@
         <v>1466</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>1467</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -27254,7 +27493,7 @@
         <v>1468</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>1469</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -27270,7 +27509,7 @@
         <v>1472</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>1473</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -27294,7 +27533,7 @@
         <v>1478</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>1479</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -27302,7 +27541,7 @@
         <v>1480</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>1481</v>
+        <v>2195</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -27334,7 +27573,7 @@
         <v>1488</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>1489</v>
+        <v>2196</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -27342,7 +27581,7 @@
         <v>1490</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>1491</v>
+        <v>2197</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -27358,7 +27597,7 @@
         <v>1494</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>1495</v>
+        <v>2198</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -27414,7 +27653,7 @@
         <v>1508</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>1509</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -27430,7 +27669,7 @@
         <v>1512</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>1513</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -27438,7 +27677,7 @@
         <v>1514</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>1515</v>
+        <v>2202</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -27446,7 +27685,7 @@
         <v>1516</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>1517</v>
+        <v>2203</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -27454,7 +27693,7 @@
         <v>1518</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>1519</v>
+        <v>2204</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -27494,7 +27733,7 @@
         <v>1528</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>1529</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -27510,7 +27749,7 @@
         <v>1532</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>1533</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -27526,7 +27765,7 @@
         <v>1536</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>1537</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -27566,7 +27805,7 @@
         <v>1546</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>1547</v>
+        <v>2208</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -27582,7 +27821,7 @@
         <v>1550</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>1551</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -27590,7 +27829,7 @@
         <v>1552</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>1553</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -27598,7 +27837,7 @@
         <v>1554</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>1555</v>
+        <v>2211</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -27606,7 +27845,7 @@
         <v>1556</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>1557</v>
+        <v>2212</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -27622,7 +27861,7 @@
         <v>1560</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>1561</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -27630,7 +27869,7 @@
         <v>1562</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>1563</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -27638,7 +27877,7 @@
         <v>1564</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>1565</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -27646,7 +27885,7 @@
         <v>1566</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>1567</v>
+        <v>2216</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -27654,7 +27893,7 @@
         <v>1568</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>1569</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -27662,7 +27901,7 @@
         <v>1570</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>1571</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -27670,7 +27909,7 @@
         <v>1572</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>1573</v>
+        <v>2219</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -27678,7 +27917,7 @@
         <v>1574</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>1575</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -27686,7 +27925,7 @@
         <v>1576</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>1577</v>
+        <v>2221</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -27694,7 +27933,7 @@
         <v>1578</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>1579</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -27702,7 +27941,7 @@
         <v>1580</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>1581</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -27710,7 +27949,7 @@
         <v>1582</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>1583</v>
+        <v>2224</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -27718,7 +27957,7 @@
         <v>1584</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>1585</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -27734,7 +27973,7 @@
         <v>1588</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>1589</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -27742,7 +27981,7 @@
         <v>1590</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>1591</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -27750,7 +27989,7 @@
         <v>1592</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>1593</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -27758,7 +27997,7 @@
         <v>1594</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>1595</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -27766,7 +28005,7 @@
         <v>1596</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>1597</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -27774,7 +28013,7 @@
         <v>1598</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>1599</v>
+        <v>2231</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -27782,7 +28021,7 @@
         <v>1600</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>1601</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -27790,7 +28029,7 @@
         <v>1602</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>1603</v>
+        <v>2233</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -27798,7 +28037,7 @@
         <v>1604</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>1605</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -27806,7 +28045,7 @@
         <v>1606</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>1607</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -27814,7 +28053,7 @@
         <v>1608</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>1609</v>
+        <v>2236</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -27830,7 +28069,7 @@
         <v>1612</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>1613</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -27838,7 +28077,7 @@
         <v>1614</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>1615</v>
+        <v>2238</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -27846,7 +28085,7 @@
         <v>1616</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>1617</v>
+        <v>2239</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -27870,7 +28109,7 @@
         <v>1622</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>1623</v>
+        <v>2240</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -27878,7 +28117,7 @@
         <v>1624</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>1625</v>
+        <v>2241</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -27886,7 +28125,7 @@
         <v>1626</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>1627</v>
+        <v>2242</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -27894,7 +28133,7 @@
         <v>1628</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>1629</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -27902,7 +28141,7 @@
         <v>1630</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>1631</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -27926,7 +28165,7 @@
         <v>1636</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>1637</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -27934,7 +28173,7 @@
         <v>1638</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>1639</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -27942,7 +28181,7 @@
         <v>1640</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>1641</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -27950,7 +28189,7 @@
         <v>1642</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>1643</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -27958,7 +28197,7 @@
         <v>1644</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>1645</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -27974,7 +28213,7 @@
         <v>1648</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>1649</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -27990,7 +28229,7 @@
         <v>1652</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>1653</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -27998,7 +28237,7 @@
         <v>1654</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>1655</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -28014,7 +28253,7 @@
         <v>1658</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>1659</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -28022,7 +28261,7 @@
         <v>1660</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>1661</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -28030,7 +28269,7 @@
         <v>1662</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>1663</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -28038,7 +28277,7 @@
         <v>1664</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>1665</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -28070,7 +28309,7 @@
         <v>1672</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>1673</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -28078,7 +28317,7 @@
         <v>1674</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>1675</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -28086,7 +28325,7 @@
         <v>1676</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>1677</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -28102,7 +28341,7 @@
         <v>1680</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>1681</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -28110,7 +28349,7 @@
         <v>1682</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>1683</v>
+        <v>2261</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -28126,7 +28365,7 @@
         <v>1686</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>1687</v>
+        <v>2262</v>
       </c>
     </row>
   </sheetData>
@@ -28146,7 +28385,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.250000"/>
   <cols>
-    <col min="4" max="4" style="1" width="17.33833334" customWidth="1" outlineLevel="0"/>
+    <col min="4" max="4" style="1" width="17.29071508" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>